<commit_message>
add hotel php file
</commit_message>
<xml_diff>
--- a/テーブルレイアウト/テーブルレイアウト 大熊.xlsx
+++ b/テーブルレイアウト/テーブルレイアウト 大熊.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\k022c0080\グループ演習\group_project\テーブルレイアウト\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po723\project\テーブルレイアウト\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C19DC8B-33E0-48EA-B96A-7511FF9F7C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37135A29-C913-45D9-9E17-AF75C2E3DB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="757" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="4185" windowWidth="21600" windowHeight="11295" tabRatio="757" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="テーブル一覧" sheetId="90" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="170">
   <si>
     <t>備考</t>
   </si>
@@ -5331,20 +5331,20 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.46484375" style="68" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="69" customWidth="1"/>
-    <col min="3" max="3" width="24.73046875" style="68" customWidth="1"/>
-    <col min="4" max="4" width="9.73046875" style="68" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="68" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="68" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="69" customWidth="1"/>
+    <col min="3" max="3" width="24.75" style="68" customWidth="1"/>
+    <col min="4" max="4" width="9.75" style="68" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="68" customWidth="1"/>
     <col min="6" max="6" width="11" style="68" customWidth="1"/>
     <col min="7" max="7" width="9" style="68"/>
-    <col min="8" max="15" width="7.1328125" style="68" customWidth="1"/>
+    <col min="8" max="15" width="7.125" style="68" customWidth="1"/>
     <col min="16" max="16384" width="9" style="68"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
@@ -5363,11 +5363,11 @@
       <c r="N1" s="2"/>
       <c r="O1" s="34"/>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B2" s="44"/>
       <c r="O2" s="35"/>
     </row>
-    <row r="3" spans="1:20" s="1" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" s="1" customFormat="1" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="64"/>
       <c r="C3" s="3"/>
@@ -5384,8 +5384,8 @@
       <c r="N3" s="4"/>
       <c r="O3" s="36"/>
     </row>
-    <row r="4" spans="1:20" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5" s="66" t="s">
         <v>30</v>
       </c>
@@ -5418,7 +5418,7 @@
       <c r="N5" s="117"/>
       <c r="O5" s="118"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6" s="54"/>
       <c r="B6" s="86" t="s">
         <v>34</v>
@@ -5437,7 +5437,7 @@
       <c r="N6" s="123"/>
       <c r="O6" s="124"/>
     </row>
-    <row r="7" spans="1:20" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="87" t="s">
         <v>35</v>
       </c>
@@ -5470,7 +5470,7 @@
       <c r="N7" s="120"/>
       <c r="O7" s="121"/>
     </row>
-    <row r="8" spans="1:20" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="87" t="s">
         <v>36</v>
       </c>
@@ -5503,7 +5503,7 @@
       <c r="N8" s="109"/>
       <c r="O8" s="110"/>
     </row>
-    <row r="9" spans="1:20" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="93" t="s">
         <v>37</v>
       </c>
@@ -5536,7 +5536,7 @@
       <c r="N9" s="120"/>
       <c r="O9" s="121"/>
     </row>
-    <row r="10" spans="1:20" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="88" t="s">
         <v>38</v>
       </c>
@@ -5574,7 +5574,7 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:20" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="87" t="s">
         <v>39</v>
       </c>
@@ -5612,7 +5612,7 @@
       <c r="S11"/>
       <c r="T11"/>
     </row>
-    <row r="12" spans="1:20" s="73" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="73" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="87" t="s">
         <v>40</v>
       </c>
@@ -5650,7 +5650,7 @@
       <c r="S12"/>
       <c r="T12"/>
     </row>
-    <row r="13" spans="1:20" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="87"/>
       <c r="B13" s="79"/>
       <c r="C13" s="89"/>
@@ -5672,7 +5672,7 @@
       <c r="S13"/>
       <c r="T13"/>
     </row>
-    <row r="14" spans="1:20" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="54"/>
       <c r="B14" s="79"/>
       <c r="C14" s="51"/>
@@ -5689,7 +5689,7 @@
       <c r="N14" s="109"/>
       <c r="O14" s="110"/>
     </row>
-    <row r="15" spans="1:20" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="87"/>
       <c r="B15" s="86"/>
       <c r="C15" s="51"/>
@@ -5706,7 +5706,7 @@
       <c r="N15" s="108"/>
       <c r="O15" s="113"/>
     </row>
-    <row r="16" spans="1:20" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="87"/>
       <c r="B16" s="81"/>
       <c r="C16" s="88"/>
@@ -5723,7 +5723,7 @@
       <c r="N16" s="109"/>
       <c r="O16" s="110"/>
     </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="87"/>
       <c r="B17" s="81"/>
       <c r="C17" s="88"/>
@@ -5740,7 +5740,7 @@
       <c r="N17" s="111"/>
       <c r="O17" s="112"/>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="87"/>
       <c r="B18" s="81"/>
       <c r="C18" s="88"/>
@@ -5757,7 +5757,7 @@
       <c r="N18" s="106"/>
       <c r="O18" s="107"/>
     </row>
-    <row r="19" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="87"/>
       <c r="B19" s="81"/>
       <c r="C19" s="88"/>
@@ -5774,7 +5774,7 @@
       <c r="N19" s="111"/>
       <c r="O19" s="112"/>
     </row>
-    <row r="20" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="87"/>
       <c r="B20" s="81"/>
       <c r="C20" s="88"/>
@@ -5791,7 +5791,7 @@
       <c r="N20" s="111"/>
       <c r="O20" s="112"/>
     </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="87"/>
       <c r="B21" s="81"/>
       <c r="C21" s="51"/>
@@ -5808,7 +5808,7 @@
       <c r="N21" s="111"/>
       <c r="O21" s="112"/>
     </row>
-    <row r="22" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="87"/>
       <c r="B22" s="81"/>
       <c r="C22" s="51"/>
@@ -5825,7 +5825,7 @@
       <c r="N22" s="111"/>
       <c r="O22" s="112"/>
     </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="87"/>
       <c r="B23" s="81"/>
       <c r="C23" s="51"/>
@@ -5842,7 +5842,7 @@
       <c r="N23" s="109"/>
       <c r="O23" s="110"/>
     </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="54"/>
       <c r="B24" s="81"/>
       <c r="C24" s="51"/>
@@ -5859,7 +5859,7 @@
       <c r="N24" s="109"/>
       <c r="O24" s="110"/>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="54"/>
       <c r="B25" s="81"/>
       <c r="C25" s="51"/>
@@ -5876,7 +5876,7 @@
       <c r="N25" s="109"/>
       <c r="O25" s="110"/>
     </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="54"/>
       <c r="B26" s="81"/>
       <c r="C26" s="51"/>
@@ -5893,7 +5893,7 @@
       <c r="N26" s="109"/>
       <c r="O26" s="110"/>
     </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="54"/>
       <c r="B27" s="81"/>
       <c r="C27" s="51"/>
@@ -5910,7 +5910,7 @@
       <c r="N27" s="109"/>
       <c r="O27" s="110"/>
     </row>
-    <row r="28" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="54"/>
       <c r="B28" s="81"/>
       <c r="C28" s="51"/>
@@ -5927,7 +5927,7 @@
       <c r="N28" s="111"/>
       <c r="O28" s="112"/>
     </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="54"/>
       <c r="B29" s="81"/>
       <c r="C29" s="51"/>
@@ -5944,7 +5944,7 @@
       <c r="N29" s="109"/>
       <c r="O29" s="110"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="54"/>
       <c r="B30" s="81"/>
       <c r="C30" s="51"/>
@@ -5961,7 +5961,7 @@
       <c r="N30" s="109"/>
       <c r="O30" s="110"/>
     </row>
-    <row r="31" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="54"/>
       <c r="B31" s="81"/>
       <c r="C31" s="51"/>
@@ -5978,7 +5978,7 @@
       <c r="N31" s="109"/>
       <c r="O31" s="110"/>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="54"/>
       <c r="B32" s="81"/>
       <c r="C32" s="51"/>
@@ -5995,7 +5995,7 @@
       <c r="N32" s="106"/>
       <c r="O32" s="107"/>
     </row>
-    <row r="33" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="54"/>
       <c r="B33" s="81"/>
       <c r="C33" s="51"/>
@@ -6012,7 +6012,7 @@
       <c r="N33" s="106"/>
       <c r="O33" s="107"/>
     </row>
-    <row r="34" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="54"/>
       <c r="B34" s="81"/>
       <c r="C34" s="51"/>
@@ -6029,7 +6029,7 @@
       <c r="N34" s="106"/>
       <c r="O34" s="107"/>
     </row>
-    <row r="35" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="54"/>
       <c r="B35" s="81"/>
       <c r="C35" s="51"/>
@@ -6046,7 +6046,7 @@
       <c r="N35" s="106"/>
       <c r="O35" s="107"/>
     </row>
-    <row r="36" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="54"/>
       <c r="B36" s="81"/>
       <c r="C36" s="51"/>
@@ -6063,7 +6063,7 @@
       <c r="N36" s="111"/>
       <c r="O36" s="112"/>
     </row>
-    <row r="37" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="54"/>
       <c r="B37" s="81"/>
       <c r="C37" s="51"/>
@@ -6080,7 +6080,7 @@
       <c r="N37" s="111"/>
       <c r="O37" s="112"/>
     </row>
-    <row r="38" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="55"/>
       <c r="B38" s="81"/>
       <c r="C38" s="56"/>
@@ -6097,10 +6097,10 @@
       <c r="N38" s="114"/>
       <c r="O38" s="115"/>
     </row>
-    <row r="39" spans="1:15" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B39" s="65"/>
     </row>
-    <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5"/>
       <c r="B40" s="69"/>
       <c r="C40" s="5"/>
@@ -6117,10 +6117,10 @@
       <c r="N40" s="5"/>
       <c r="O40" s="37"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B41" s="5"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="H44" s="68" t="s">
         <v>20</v>
       </c>
@@ -6177,31 +6177,31 @@
   </sheetPr>
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
     <col min="10" max="14" width="3" style="1" customWidth="1"/>
-    <col min="15" max="15" width="44.86328125" style="35" customWidth="1"/>
-    <col min="16" max="16" width="8.86328125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="26.73046875" style="71" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="61.46484375" style="71" customWidth="1"/>
-    <col min="19" max="19" width="61.46484375" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.86328125" style="1"/>
+    <col min="15" max="15" width="44.875" style="35" customWidth="1"/>
+    <col min="16" max="16" width="8.875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="26.75" style="71" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="61.5" style="71" customWidth="1"/>
+    <col min="19" max="19" width="61.5" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
@@ -6220,8 +6220,8 @@
       <c r="N1" s="2"/>
       <c r="O1" s="34"/>
     </row>
-    <row r="2" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:18" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6238,8 +6238,8 @@
       <c r="N3" s="4"/>
       <c r="O3" s="36"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="125" t="s">
         <v>1</v>
       </c>
@@ -6270,7 +6270,7 @@
       <c r="N5" s="126"/>
       <c r="O5" s="128"/>
     </row>
-    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="129" t="s">
         <v>45</v>
       </c>
@@ -6301,8 +6301,8 @@
       <c r="N6" s="132"/>
       <c r="O6" s="133"/>
     </row>
-    <row r="7" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="134" t="s">
         <v>2</v>
       </c>
@@ -6341,7 +6341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="78" customFormat="1" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="78" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="135"/>
       <c r="B9" s="137"/>
       <c r="C9" s="137"/>
@@ -6371,7 +6371,7 @@
       <c r="Q9" s="77"/>
       <c r="R9" s="77"/>
     </row>
-    <row r="10" spans="1:18" ht="13.15" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A10" s="30">
         <v>1</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>/* 予約情報ID   yyyymm+ユーザーID+連番3桁 */</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>2</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>/* ユーザーID    */</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>3</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>/* プランID    */</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>4</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>/* 予約日    */</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>5</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>/* 宿泊開始日    */</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="15">
         <v>6</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>/* 宿泊終了日    */</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="15">
         <v>7</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="15">
         <v>8</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="15">
         <v>9</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="15">
         <v>10</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="15">
         <v>11</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="15">
         <v>12</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="15">
         <v>13</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="15">
         <v>14</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="15">
         <v>15</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="15">
         <v>16</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="15">
         <v>17</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="15">
         <v>18</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="15">
         <v>19</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="15">
         <v>20</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="15">
         <v>21</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="15">
         <v>22</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="15">
         <v>23</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33" s="15">
         <v>24</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="15">
         <v>25</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="15">
         <v>26</v>
       </c>
@@ -7225,7 +7225,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="15">
         <v>27</v>
       </c>
@@ -7257,7 +7257,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="15">
         <v>28</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="15">
         <v>29</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="15">
         <v>30</v>
       </c>
@@ -7353,7 +7353,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="15">
         <v>31</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A41" s="15">
         <v>32</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42" s="15">
         <v>33</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" s="15">
         <v>34</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="16">
         <v>35</v>
       </c>
@@ -7511,19 +7511,19 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R45" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R46" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -7544,25 +7544,25 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R48" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="49" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R49" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="50" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R50" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="51" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R51" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
@@ -7607,27 +7607,27 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.86328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
     <col min="10" max="14" width="3" style="1" customWidth="1"/>
-    <col min="15" max="15" width="44.86328125" style="35" customWidth="1"/>
-    <col min="16" max="16" width="8.86328125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="26.73046875" style="71" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="61.46484375" style="71" customWidth="1"/>
-    <col min="19" max="19" width="61.46484375" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.86328125" style="1"/>
+    <col min="15" max="15" width="44.875" style="35" customWidth="1"/>
+    <col min="16" max="16" width="8.875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="26.75" style="71" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="61.5" style="71" customWidth="1"/>
+    <col min="19" max="19" width="61.5" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
@@ -7646,8 +7646,8 @@
       <c r="N1" s="2"/>
       <c r="O1" s="34"/>
     </row>
-    <row r="2" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:18" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -7664,8 +7664,8 @@
       <c r="N3" s="4"/>
       <c r="O3" s="36"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="125" t="s">
         <v>1</v>
       </c>
@@ -7696,7 +7696,7 @@
       <c r="N5" s="126"/>
       <c r="O5" s="128"/>
     </row>
-    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="129" t="s">
         <v>46</v>
       </c>
@@ -7727,8 +7727,8 @@
       <c r="N6" s="132"/>
       <c r="O6" s="133"/>
     </row>
-    <row r="7" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="134" t="s">
         <v>2</v>
       </c>
@@ -7767,7 +7767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="78" customFormat="1" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="78" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="135"/>
       <c r="B9" s="137"/>
       <c r="C9" s="137"/>
@@ -7797,7 +7797,7 @@
       <c r="Q9" s="77"/>
       <c r="R9" s="77"/>
     </row>
-    <row r="10" spans="1:18" ht="13.15" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A10" s="30">
         <v>1</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>/* 口コミID   連番10桁 */</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>2</v>
       </c>
@@ -7881,7 +7881,7 @@
         <v>/* ユーザーID   記入したユーザーのID */</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>3</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>/* ホテルID   記入されたホテルのID */</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>4</v>
       </c>
@@ -7963,7 +7963,7 @@
         <v>/* 口コミ日    */</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>5</v>
       </c>
@@ -8005,7 +8005,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="15">
         <v>6</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>/* 口コミ内容   1～5の五段階評価 */</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="15">
         <v>7</v>
       </c>
@@ -8077,7 +8077,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="15">
         <v>8</v>
       </c>
@@ -8107,7 +8107,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="15">
         <v>9</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="15">
         <v>10</v>
       </c>
@@ -8167,7 +8167,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="15">
         <v>11</v>
       </c>
@@ -8197,7 +8197,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="15">
         <v>12</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="15">
         <v>13</v>
       </c>
@@ -8257,7 +8257,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="15">
         <v>14</v>
       </c>
@@ -8287,7 +8287,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="15">
         <v>15</v>
       </c>
@@ -8317,7 +8317,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="15">
         <v>16</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="15">
         <v>17</v>
       </c>
@@ -8377,7 +8377,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="15">
         <v>18</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="15">
         <v>19</v>
       </c>
@@ -8437,7 +8437,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="15">
         <v>20</v>
       </c>
@@ -8467,7 +8467,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="15">
         <v>21</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="15">
         <v>22</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="15">
         <v>23</v>
       </c>
@@ -8563,7 +8563,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33" s="15">
         <v>24</v>
       </c>
@@ -8595,7 +8595,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="15">
         <v>25</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="15">
         <v>26</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="15">
         <v>27</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="15">
         <v>28</v>
       </c>
@@ -8723,7 +8723,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="15">
         <v>29</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="15">
         <v>30</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="15">
         <v>31</v>
       </c>
@@ -8819,7 +8819,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A41" s="15">
         <v>32</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42" s="15">
         <v>33</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" s="15">
         <v>34</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="16">
         <v>35</v>
       </c>
@@ -8945,19 +8945,19 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R45" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R46" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -8978,25 +8978,25 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R48" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="49" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R49" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="50" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R50" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="51" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R51" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
@@ -9037,31 +9037,31 @@
   </sheetPr>
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="25.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.46484375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
     <col min="10" max="14" width="3" style="1" customWidth="1"/>
-    <col min="15" max="15" width="44.86328125" style="44" customWidth="1"/>
-    <col min="16" max="16" width="8.86328125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.73046875" style="71" customWidth="1"/>
-    <col min="18" max="18" width="8.86328125" style="71" customWidth="1"/>
-    <col min="19" max="19" width="8.86328125" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.86328125" style="1"/>
+    <col min="15" max="15" width="44.875" style="44" customWidth="1"/>
+    <col min="16" max="16" width="8.875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.75" style="71" customWidth="1"/>
+    <col min="18" max="18" width="8.875" style="71" customWidth="1"/>
+    <col min="19" max="19" width="8.875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
@@ -9080,8 +9080,8 @@
       <c r="N1" s="2"/>
       <c r="O1" s="43"/>
     </row>
-    <row r="2" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:18" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="38"/>
       <c r="C3" s="3"/>
@@ -9098,8 +9098,8 @@
       <c r="N3" s="4"/>
       <c r="O3" s="45"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="125" t="s">
         <v>1</v>
       </c>
@@ -9130,7 +9130,7 @@
       <c r="N5" s="142"/>
       <c r="O5" s="143"/>
     </row>
-    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="144" t="s">
         <v>48</v>
       </c>
@@ -9161,8 +9161,8 @@
       <c r="N6" s="146"/>
       <c r="O6" s="147"/>
     </row>
-    <row r="7" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="134" t="s">
         <v>2</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="78" customFormat="1" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="78" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="135"/>
       <c r="B9" s="137"/>
       <c r="C9" s="137"/>
@@ -9231,7 +9231,7 @@
       <c r="Q9" s="77"/>
       <c r="R9" s="77"/>
     </row>
-    <row r="10" spans="1:18" ht="13.15" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A10" s="30">
         <v>1</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>/* ホテルID   県番号(2桁)+連番8 */</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>2</v>
       </c>
@@ -9313,7 +9313,7 @@
         <v>/* 住所    */</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>3</v>
       </c>
@@ -9353,7 +9353,7 @@
         <v>/* メールアドレス    */</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>4</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>/* 電話番号   ハイフンは抜く */</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>5</v>
       </c>
@@ -9435,7 +9435,7 @@
         <v>/* 建物名    */</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="15">
         <v>6</v>
       </c>
@@ -9475,7 +9475,7 @@
         <v>/* ホテル名    */</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="15">
         <v>7</v>
       </c>
@@ -9517,7 +9517,7 @@
         <v>/* ホテル写真   images/配下に写真を置く images/〇〇〇 */</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="15">
         <v>8</v>
       </c>
@@ -9528,7 +9528,7 @@
         <v>152</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>67</v>
+        <v>140</v>
       </c>
       <c r="E17" s="102">
         <v>1200</v>
@@ -9548,19 +9548,23 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="71" t="str">
         <f t="shared" si="0"/>
-        <v>HOTEL_EXPLAIN CHAR(1200)</v>
+        <v>HOTEL_EXPLAIN TEXT(1200)</v>
       </c>
       <c r="R17" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/* ホテル説明    */</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="15">
         <v>9</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="24"/>
+      <c r="B18" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>168</v>
+      </c>
       <c r="D18" s="32"/>
       <c r="E18" s="102"/>
       <c r="F18" s="24"/>
@@ -9574,8 +9578,12 @@
       <c r="N18" s="26"/>
       <c r="O18" s="46"/>
       <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R18" s="71" t="str">
+        <f t="shared" si="1"/>
+        <v>/* 郵便番号    */</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="15"/>
       <c r="B19" s="40"/>
       <c r="C19" s="24"/>
@@ -9593,7 +9601,7 @@
       <c r="O19" s="46"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="15"/>
       <c r="B20" s="40"/>
       <c r="C20" s="24"/>
@@ -9611,7 +9619,7 @@
       <c r="O20" s="46"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="15"/>
       <c r="B21" s="40"/>
       <c r="C21" s="24"/>
@@ -9629,7 +9637,7 @@
       <c r="O21" s="46"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="15">
         <v>13</v>
       </c>
@@ -9659,7 +9667,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="15">
         <v>14</v>
       </c>
@@ -9689,7 +9697,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="15">
         <v>15</v>
       </c>
@@ -9719,7 +9727,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="15">
         <v>16</v>
       </c>
@@ -9749,7 +9757,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="15">
         <v>17</v>
       </c>
@@ -9779,7 +9787,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="15">
         <v>18</v>
       </c>
@@ -9809,7 +9817,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="15">
         <v>19</v>
       </c>
@@ -9839,7 +9847,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="15">
         <v>20</v>
       </c>
@@ -9869,7 +9877,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="15">
         <v>21</v>
       </c>
@@ -9899,7 +9907,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="15">
         <v>22</v>
       </c>
@@ -9929,7 +9937,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="15">
         <v>23</v>
       </c>
@@ -9959,7 +9967,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33" s="15">
         <v>24</v>
       </c>
@@ -9989,7 +9997,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="15">
         <v>25</v>
       </c>
@@ -10019,7 +10027,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="15">
         <v>26</v>
       </c>
@@ -10049,7 +10057,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="15">
         <v>27</v>
       </c>
@@ -10079,7 +10087,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="15">
         <v>28</v>
       </c>
@@ -10109,7 +10117,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="15">
         <v>29</v>
       </c>
@@ -10139,7 +10147,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="15">
         <v>30</v>
       </c>
@@ -10169,7 +10177,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="15">
         <v>31</v>
       </c>
@@ -10199,7 +10207,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16">
         <v>32</v>
       </c>
@@ -10229,7 +10237,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="P42" s="6" t="s">
         <v>29</v>
       </c>
@@ -10242,7 +10250,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="P43" s="6" t="s">
         <v>29</v>
       </c>
@@ -10255,7 +10263,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="5"/>
       <c r="B44" s="37"/>
       <c r="C44" s="5"/>
@@ -10276,37 +10284,37 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R45" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R46" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R47" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R48" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="49" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R49" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="50" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R50" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
@@ -10351,27 +10359,27 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="25.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.46484375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
     <col min="10" max="14" width="3" style="1" customWidth="1"/>
-    <col min="15" max="15" width="44.86328125" style="44" customWidth="1"/>
-    <col min="16" max="16" width="8.86328125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.73046875" style="71" customWidth="1"/>
-    <col min="18" max="18" width="8.86328125" style="71" customWidth="1"/>
-    <col min="19" max="19" width="8.86328125" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.86328125" style="1"/>
+    <col min="15" max="15" width="44.875" style="44" customWidth="1"/>
+    <col min="16" max="16" width="8.875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.75" style="71" customWidth="1"/>
+    <col min="18" max="18" width="8.875" style="71" customWidth="1"/>
+    <col min="19" max="19" width="8.875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
@@ -10390,8 +10398,8 @@
       <c r="N1" s="2"/>
       <c r="O1" s="43"/>
     </row>
-    <row r="2" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:18" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="38"/>
       <c r="C3" s="3"/>
@@ -10408,8 +10416,8 @@
       <c r="N3" s="4"/>
       <c r="O3" s="45"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="125" t="s">
         <v>1</v>
       </c>
@@ -10440,7 +10448,7 @@
       <c r="N5" s="142"/>
       <c r="O5" s="143"/>
     </row>
-    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="144" t="s">
         <v>47</v>
       </c>
@@ -10471,8 +10479,8 @@
       <c r="N6" s="146"/>
       <c r="O6" s="147"/>
     </row>
-    <row r="7" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="134" t="s">
         <v>2</v>
       </c>
@@ -10511,7 +10519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="78" customFormat="1" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="78" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="135"/>
       <c r="B9" s="137"/>
       <c r="C9" s="137"/>
@@ -10541,7 +10549,7 @@
       <c r="Q9" s="77"/>
       <c r="R9" s="77"/>
     </row>
-    <row r="10" spans="1:18" ht="13.15" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A10" s="30">
         <v>1</v>
       </c>
@@ -10583,7 +10591,7 @@
         <v>/* プランID   ホテルID＋1+連番3桁 */</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>2</v>
       </c>
@@ -10623,7 +10631,7 @@
         <v>/* プラン名    */</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>3</v>
       </c>
@@ -10663,7 +10671,7 @@
         <v>/* 最大人数    */</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>4</v>
       </c>
@@ -10703,7 +10711,7 @@
         <v>/* ホテルID    */</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>5</v>
       </c>
@@ -10743,7 +10751,7 @@
         <v>/* 料金    */</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="15">
         <v>6</v>
       </c>
@@ -10783,7 +10791,7 @@
         <v>/* 部屋ID    */</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="15"/>
       <c r="B16" s="40" t="s">
         <v>144</v>
@@ -10819,7 +10827,7 @@
         <v>/* プラン説明    */</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="15"/>
       <c r="B17" s="40" t="s">
         <v>154</v>
@@ -10853,7 +10861,7 @@
         <v>/* 子供料金    */</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="15"/>
       <c r="B18" s="40" t="s">
         <v>155</v>
@@ -10887,7 +10895,7 @@
         <v>/* 乳幼児料金    */</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="15"/>
       <c r="B19" s="40"/>
       <c r="C19" s="24"/>
@@ -10905,7 +10913,7 @@
       <c r="O19" s="46"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="15"/>
       <c r="B20" s="40"/>
       <c r="C20" s="24"/>
@@ -10923,7 +10931,7 @@
       <c r="O20" s="46"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="15"/>
       <c r="B21" s="40"/>
       <c r="C21" s="24"/>
@@ -10941,7 +10949,7 @@
       <c r="O21" s="46"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="15"/>
       <c r="B22" s="40"/>
       <c r="C22" s="24"/>
@@ -10969,7 +10977,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="15"/>
       <c r="B23" s="40"/>
       <c r="C23" s="24"/>
@@ -10997,7 +11005,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="15"/>
       <c r="B24" s="40"/>
       <c r="C24" s="24"/>
@@ -11025,7 +11033,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="15"/>
       <c r="B25" s="40"/>
       <c r="C25" s="24"/>
@@ -11053,7 +11061,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="15"/>
       <c r="B26" s="40"/>
       <c r="C26" s="24"/>
@@ -11081,7 +11089,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="15"/>
       <c r="B27" s="40"/>
       <c r="C27" s="24"/>
@@ -11109,7 +11117,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="15"/>
       <c r="B28" s="40"/>
       <c r="C28" s="24"/>
@@ -11137,7 +11145,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="15"/>
       <c r="B29" s="39"/>
       <c r="C29" s="29"/>
@@ -11165,7 +11173,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="15"/>
       <c r="B30" s="39"/>
       <c r="C30" s="29"/>
@@ -11193,7 +11201,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="15"/>
       <c r="B31" s="39"/>
       <c r="C31" s="29"/>
@@ -11221,7 +11229,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="15"/>
       <c r="B32" s="9"/>
       <c r="C32" s="24"/>
@@ -11249,7 +11257,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33" s="15"/>
       <c r="B33" s="40"/>
       <c r="C33" s="24"/>
@@ -11277,7 +11285,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="15"/>
       <c r="B34" s="40"/>
       <c r="C34" s="24"/>
@@ -11305,7 +11313,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="15"/>
       <c r="B35" s="40"/>
       <c r="C35" s="24"/>
@@ -11333,7 +11341,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="15"/>
       <c r="B36" s="40"/>
       <c r="C36" s="24"/>
@@ -11361,7 +11369,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="15"/>
       <c r="B37" s="40"/>
       <c r="C37" s="24"/>
@@ -11389,7 +11397,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="15"/>
       <c r="B38" s="40"/>
       <c r="C38" s="24"/>
@@ -11417,7 +11425,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="15"/>
       <c r="B39" s="40"/>
       <c r="C39" s="24"/>
@@ -11445,7 +11453,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="15"/>
       <c r="B40" s="40"/>
       <c r="C40" s="24"/>
@@ -11473,7 +11481,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16"/>
       <c r="B41" s="41"/>
       <c r="C41" s="14"/>
@@ -11501,7 +11509,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="P42" s="6" t="s">
         <v>29</v>
       </c>
@@ -11514,7 +11522,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="P43" s="6" t="s">
         <v>29</v>
       </c>
@@ -11527,7 +11535,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="5"/>
       <c r="B44" s="37"/>
       <c r="C44" s="5"/>
@@ -11548,37 +11556,37 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R45" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R46" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R47" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R48" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="49" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R49" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="50" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R50" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
@@ -11620,27 +11628,27 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="25.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.46484375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
     <col min="10" max="14" width="3" style="1" customWidth="1"/>
-    <col min="15" max="15" width="44.86328125" style="44" customWidth="1"/>
-    <col min="16" max="16" width="8.86328125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.73046875" style="71" customWidth="1"/>
-    <col min="18" max="18" width="8.86328125" style="71" customWidth="1"/>
-    <col min="19" max="19" width="8.86328125" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.86328125" style="1"/>
+    <col min="15" max="15" width="44.875" style="44" customWidth="1"/>
+    <col min="16" max="16" width="8.875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.75" style="71" customWidth="1"/>
+    <col min="18" max="18" width="8.875" style="71" customWidth="1"/>
+    <col min="19" max="19" width="8.875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
@@ -11659,8 +11667,8 @@
       <c r="N1" s="2"/>
       <c r="O1" s="43"/>
     </row>
-    <row r="2" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:18" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="38"/>
       <c r="C3" s="3"/>
@@ -11677,8 +11685,8 @@
       <c r="N3" s="4"/>
       <c r="O3" s="45"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="125" t="s">
         <v>1</v>
       </c>
@@ -11709,7 +11717,7 @@
       <c r="N5" s="142"/>
       <c r="O5" s="143"/>
     </row>
-    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="144" t="s">
         <v>49</v>
       </c>
@@ -11740,8 +11748,8 @@
       <c r="N6" s="146"/>
       <c r="O6" s="147"/>
     </row>
-    <row r="7" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="134" t="s">
         <v>2</v>
       </c>
@@ -11780,7 +11788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="78" customFormat="1" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="78" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="135"/>
       <c r="B9" s="137"/>
       <c r="C9" s="137"/>
@@ -11810,7 +11818,7 @@
       <c r="Q9" s="77"/>
       <c r="R9" s="77"/>
     </row>
-    <row r="10" spans="1:18" ht="13.15" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A10" s="30">
         <v>1</v>
       </c>
@@ -11852,7 +11860,7 @@
         <v>/* 部屋ID   ホテルID＋2+連番3桁 */</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>2</v>
       </c>
@@ -11892,7 +11900,7 @@
         <v>/* 冷蔵庫    */</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>3</v>
       </c>
@@ -11932,7 +11940,7 @@
         <v>/* ベッド数    */</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>4</v>
       </c>
@@ -11972,7 +11980,7 @@
         <v>/* バスルーム    */</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>5</v>
       </c>
@@ -12012,7 +12020,7 @@
         <v>/* ドライヤー    */</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="15">
         <v>6</v>
       </c>
@@ -12052,7 +12060,7 @@
         <v>/* テレビ    */</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="15">
         <v>7</v>
       </c>
@@ -12092,7 +12100,7 @@
         <v>/* WIFI    */</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="15">
         <v>8</v>
       </c>
@@ -12130,7 +12138,7 @@
         <v>/* ペット    */</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="15">
         <v>9</v>
       </c>
@@ -12170,7 +12178,7 @@
         <v>/* 部屋写真   images/配下に写真を置く images/〇〇〇 */</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="15">
         <v>10</v>
       </c>
@@ -12190,7 +12198,7 @@
       <c r="O19" s="46"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="15">
         <v>11</v>
       </c>
@@ -12210,7 +12218,7 @@
       <c r="O20" s="46"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="15">
         <v>12</v>
       </c>
@@ -12230,7 +12238,7 @@
       <c r="O21" s="46"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="15">
         <v>13</v>
       </c>
@@ -12260,7 +12268,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="15">
         <v>14</v>
       </c>
@@ -12290,7 +12298,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="15">
         <v>15</v>
       </c>
@@ -12320,7 +12328,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="15">
         <v>16</v>
       </c>
@@ -12350,7 +12358,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="15">
         <v>17</v>
       </c>
@@ -12380,7 +12388,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="15">
         <v>18</v>
       </c>
@@ -12410,7 +12418,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="15">
         <v>19</v>
       </c>
@@ -12440,7 +12448,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="15">
         <v>20</v>
       </c>
@@ -12470,7 +12478,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="15">
         <v>21</v>
       </c>
@@ -12500,7 +12508,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="15">
         <v>22</v>
       </c>
@@ -12530,7 +12538,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="15">
         <v>23</v>
       </c>
@@ -12560,7 +12568,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33" s="15">
         <v>24</v>
       </c>
@@ -12590,7 +12598,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="15">
         <v>25</v>
       </c>
@@ -12620,7 +12628,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="15">
         <v>26</v>
       </c>
@@ -12650,7 +12658,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="15">
         <v>27</v>
       </c>
@@ -12680,7 +12688,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="15">
         <v>28</v>
       </c>
@@ -12710,7 +12718,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="15">
         <v>29</v>
       </c>
@@ -12740,7 +12748,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="15">
         <v>30</v>
       </c>
@@ -12770,7 +12778,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="15">
         <v>31</v>
       </c>
@@ -12800,7 +12808,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16">
         <v>32</v>
       </c>
@@ -12830,7 +12838,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="P42" s="6" t="s">
         <v>29</v>
       </c>
@@ -12843,7 +12851,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="P43" s="6" t="s">
         <v>29</v>
       </c>
@@ -12856,7 +12864,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="5"/>
       <c r="B44" s="37"/>
       <c r="C44" s="5"/>
@@ -12877,37 +12885,37 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R45" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R46" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R47" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R48" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="49" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R49" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="50" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R50" s="71" t="str">
         <f t="shared" si="1"/>
         <v>/*     */</v>
@@ -12949,30 +12957,30 @@
   <dimension ref="A1:R50"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B21" sqref="B21:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="25.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.46484375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
     <col min="10" max="14" width="3" style="1" customWidth="1"/>
-    <col min="15" max="15" width="44.86328125" style="44" customWidth="1"/>
-    <col min="16" max="16" width="8.86328125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.73046875" style="71" customWidth="1"/>
-    <col min="18" max="18" width="8.86328125" style="71" customWidth="1"/>
-    <col min="19" max="19" width="8.86328125" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.86328125" style="1"/>
+    <col min="15" max="15" width="44.875" style="44" customWidth="1"/>
+    <col min="16" max="16" width="8.875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.75" style="71" customWidth="1"/>
+    <col min="18" max="18" width="8.875" style="71" customWidth="1"/>
+    <col min="19" max="19" width="8.875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
@@ -12991,8 +12999,8 @@
       <c r="N1" s="2"/>
       <c r="O1" s="43"/>
     </row>
-    <row r="2" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:18" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="38"/>
       <c r="C3" s="3"/>
@@ -13009,8 +13017,8 @@
       <c r="N3" s="4"/>
       <c r="O3" s="45"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="125" t="s">
         <v>1</v>
       </c>
@@ -13041,7 +13049,7 @@
       <c r="N5" s="142"/>
       <c r="O5" s="143"/>
     </row>
-    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="144" t="s">
         <v>44</v>
       </c>
@@ -13072,8 +13080,8 @@
       <c r="N6" s="146"/>
       <c r="O6" s="147"/>
     </row>
-    <row r="7" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="134" t="s">
         <v>2</v>
       </c>
@@ -13112,7 +13120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="78" customFormat="1" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="78" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="135"/>
       <c r="B9" s="137"/>
       <c r="C9" s="137"/>
@@ -13142,7 +13150,7 @@
       <c r="Q9" s="77"/>
       <c r="R9" s="77"/>
     </row>
-    <row r="10" spans="1:18" ht="13.15" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15">
         <v>5</v>
       </c>
@@ -13186,7 +13194,7 @@
         <v>/* ユーザーID   UR＋連番８文字 */</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>2</v>
       </c>
@@ -13226,7 +13234,7 @@
         <v>/* ユーザーパスワード    */</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>3</v>
       </c>
@@ -13266,7 +13274,7 @@
         <v>/* メールアドレス    */</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>4</v>
       </c>
@@ -13306,7 +13314,7 @@
         <v>/* 住所    */</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>7</v>
       </c>
@@ -13350,7 +13358,7 @@
         <v>/* ロール   1→会員　2→ホテル　3→管理者　0→ログインしていない */</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="30">
         <v>1</v>
       </c>
@@ -13390,7 +13398,7 @@
         <v>/* 名前   日本語なら25文字 */</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="15"/>
       <c r="B16" s="40" t="s">
         <v>104</v>
@@ -13424,7 +13432,7 @@
         <v>PHONE_NUMBER INT(20)</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="15"/>
       <c r="B17" s="40" t="s">
         <v>159</v>
@@ -13458,7 +13466,7 @@
         <v>BIRTHDAY VARCHAR(20)</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="15"/>
       <c r="B18" s="40" t="s">
         <v>161</v>
@@ -13488,7 +13496,7 @@
       </c>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="15"/>
       <c r="B19" s="40" t="s">
         <v>164</v>
@@ -13518,7 +13526,7 @@
       </c>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="15"/>
       <c r="B20" s="40" t="s">
         <v>58</v>
@@ -13540,7 +13548,7 @@
       <c r="O20" s="46"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="15"/>
       <c r="B21" s="40" t="s">
         <v>166</v>
@@ -13562,7 +13570,7 @@
       <c r="O21" s="46"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="15">
         <v>13</v>
       </c>
@@ -13592,7 +13600,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="15">
         <v>14</v>
       </c>
@@ -13622,7 +13630,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="15">
         <v>15</v>
       </c>
@@ -13652,7 +13660,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="15">
         <v>16</v>
       </c>
@@ -13682,7 +13690,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="15">
         <v>17</v>
       </c>
@@ -13712,7 +13720,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="15">
         <v>18</v>
       </c>
@@ -13742,7 +13750,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="15">
         <v>19</v>
       </c>
@@ -13772,7 +13780,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="15">
         <v>20</v>
       </c>
@@ -13802,7 +13810,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="15">
         <v>21</v>
       </c>
@@ -13832,7 +13840,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="15">
         <v>22</v>
       </c>
@@ -13862,7 +13870,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="15">
         <v>23</v>
       </c>
@@ -13892,7 +13900,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33" s="15">
         <v>24</v>
       </c>
@@ -13922,7 +13930,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="15">
         <v>25</v>
       </c>
@@ -13952,7 +13960,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="15">
         <v>26</v>
       </c>
@@ -13982,7 +13990,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="15">
         <v>27</v>
       </c>
@@ -14012,7 +14020,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="15">
         <v>28</v>
       </c>
@@ -14042,7 +14050,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="15">
         <v>29</v>
       </c>
@@ -14072,7 +14080,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="15">
         <v>30</v>
       </c>
@@ -14102,7 +14110,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="15">
         <v>31</v>
       </c>
@@ -14132,7 +14140,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16">
         <v>32</v>
       </c>
@@ -14162,7 +14170,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="P42" s="6" t="s">
         <v>29</v>
       </c>
@@ -14175,7 +14183,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="P43" s="6" t="s">
         <v>29</v>
       </c>
@@ -14188,7 +14196,7 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="5"/>
       <c r="B44" s="37"/>
       <c r="C44" s="5"/>
@@ -14209,37 +14217,37 @@
         <v>/*     */</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R45" s="71" t="str">
         <f t="shared" si="2"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R46" s="71" t="str">
         <f t="shared" si="2"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R47" s="71" t="str">
         <f t="shared" si="2"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="R48" s="71" t="str">
         <f t="shared" si="2"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="49" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R49" s="71" t="str">
         <f t="shared" si="2"/>
         <v>/*     */</v>
       </c>
     </row>
-    <row r="50" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="18:18" x14ac:dyDescent="0.15">
       <c r="R50" s="71" t="str">
         <f t="shared" si="2"/>
         <v>/*     */</v>

</xml_diff>